<commit_message>
Atualização BD e planilhas
</commit_message>
<xml_diff>
--- a/Backlog Sprint.xlsx
+++ b/Backlog Sprint.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vini\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pi\PI-1o-semestre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87D21CA-0C28-4EE6-941E-EA64CA783D15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D7CD22-6293-425F-ABCB-84EAAE95CCB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{15C77D7C-C8EB-4137-B167-53689B4808DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{15C77D7C-C8EB-4137-B167-53689B4808DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -592,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -606,9 +606,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -633,6 +630,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -681,76 +682,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -768,20 +736,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1100,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B20147F5-1783-4C3D-8F98-0699CC9A293A}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,40 +1109,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="39" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="61" t="s">
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="38" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="62"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="57"/>
       <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1155,567 +1152,567 @@
       <c r="G3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="63"/>
+      <c r="J3" s="40"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="64"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="43"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="7">
+      <c r="A5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="6">
         <v>3</v>
       </c>
-      <c r="F5" s="7">
-        <v>5</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="F5" s="6">
+        <v>5</v>
+      </c>
+      <c r="G5" s="6">
         <v>3</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <v>3</v>
       </c>
-      <c r="I5" s="7">
-        <v>8</v>
-      </c>
-      <c r="J5" s="59">
-        <v>5</v>
-      </c>
-      <c r="K5" s="60"/>
+      <c r="I5" s="6">
+        <v>8</v>
+      </c>
+      <c r="J5" s="13">
+        <v>5</v>
+      </c>
+      <c r="K5" s="14"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="8">
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="7">
         <v>3</v>
       </c>
-      <c r="F6" s="8">
-        <v>5</v>
-      </c>
-      <c r="G6" s="8">
+      <c r="F6" s="7">
+        <v>5</v>
+      </c>
+      <c r="G6" s="7">
         <v>3</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <v>3</v>
       </c>
-      <c r="I6" s="8">
-        <v>5</v>
-      </c>
-      <c r="J6" s="59">
-        <v>5</v>
-      </c>
-      <c r="K6" s="60"/>
+      <c r="I6" s="7">
+        <v>5</v>
+      </c>
+      <c r="J6" s="13">
+        <v>5</v>
+      </c>
+      <c r="K6" s="14"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="9">
-        <v>8</v>
-      </c>
-      <c r="F7" s="9">
-        <v>8</v>
-      </c>
-      <c r="G7" s="9">
-        <v>5</v>
-      </c>
-      <c r="H7" s="9">
-        <v>8</v>
-      </c>
-      <c r="I7" s="9">
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="8">
+        <v>8</v>
+      </c>
+      <c r="F7" s="8">
+        <v>8</v>
+      </c>
+      <c r="G7" s="8">
+        <v>5</v>
+      </c>
+      <c r="H7" s="8">
+        <v>8</v>
+      </c>
+      <c r="I7" s="8">
         <v>13</v>
       </c>
-      <c r="J7" s="59">
-        <v>8</v>
-      </c>
-      <c r="K7" s="60"/>
+      <c r="J7" s="13">
+        <v>8</v>
+      </c>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
     </row>
     <row r="9" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="64"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="43"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="7">
-        <v>8</v>
-      </c>
-      <c r="F10" s="7">
-        <v>8</v>
-      </c>
-      <c r="G10" s="7">
-        <v>5</v>
-      </c>
-      <c r="H10" s="7">
+      <c r="A10" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="6">
+        <v>8</v>
+      </c>
+      <c r="F10" s="6">
+        <v>8</v>
+      </c>
+      <c r="G10" s="6">
+        <v>5</v>
+      </c>
+      <c r="H10" s="6">
         <v>3</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <v>3</v>
       </c>
-      <c r="J10" s="59">
+      <c r="J10" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="8">
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="7">
+        <v>8</v>
+      </c>
+      <c r="F11" s="7">
         <v>13</v>
       </c>
-      <c r="F11" s="8">
+      <c r="G11" s="7">
+        <v>5</v>
+      </c>
+      <c r="H11" s="7">
+        <v>5</v>
+      </c>
+      <c r="I11" s="7">
+        <v>5</v>
+      </c>
+      <c r="J11" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="8">
+        <v>8</v>
+      </c>
+      <c r="F12" s="8">
+        <v>8</v>
+      </c>
+      <c r="G12" s="8">
+        <v>8</v>
+      </c>
+      <c r="H12" s="8">
+        <v>3</v>
+      </c>
+      <c r="I12" s="8">
+        <v>3</v>
+      </c>
+      <c r="J12" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="44"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+    </row>
+    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="43"/>
+    </row>
+    <row r="15" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="8">
-        <v>5</v>
-      </c>
-      <c r="H11" s="8">
-        <v>5</v>
-      </c>
-      <c r="I11" s="8">
-        <v>5</v>
-      </c>
-      <c r="J11" s="59">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="9">
-        <v>8</v>
-      </c>
-      <c r="F12" s="9">
-        <v>8</v>
-      </c>
-      <c r="G12" s="9">
-        <v>8</v>
-      </c>
-      <c r="H12" s="9">
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="6">
+        <v>5</v>
+      </c>
+      <c r="F15" s="6">
+        <v>8</v>
+      </c>
+      <c r="G15" s="6">
         <v>3</v>
       </c>
-      <c r="I12" s="9">
+      <c r="H15" s="6">
         <v>3</v>
       </c>
-      <c r="J12" s="59">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="54"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-    </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="64"/>
-    </row>
-    <row r="15" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="56" t="s">
+      <c r="I15" s="6">
+        <v>8</v>
+      </c>
+      <c r="J15" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="7">
+        <v>8</v>
+      </c>
+      <c r="F16" s="7">
         <v>13</v>
       </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="7">
-        <v>5</v>
-      </c>
-      <c r="F15" s="7">
-        <v>8</v>
-      </c>
-      <c r="G15" s="7">
+      <c r="G16" s="7">
+        <v>5</v>
+      </c>
+      <c r="H16" s="7">
+        <v>8</v>
+      </c>
+      <c r="I16" s="7">
+        <v>13</v>
+      </c>
+      <c r="J16" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="8">
+        <v>5</v>
+      </c>
+      <c r="F17" s="8">
+        <v>8</v>
+      </c>
+      <c r="G17" s="8">
+        <v>8</v>
+      </c>
+      <c r="H17" s="8">
+        <v>8</v>
+      </c>
+      <c r="I17" s="8">
+        <v>5</v>
+      </c>
+      <c r="J17" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="44"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+    </row>
+    <row r="19" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="43"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="9">
+        <v>8</v>
+      </c>
+      <c r="F20" s="6">
+        <v>5</v>
+      </c>
+      <c r="G20" s="6">
         <v>3</v>
       </c>
-      <c r="H15" s="7">
-        <v>3</v>
-      </c>
-      <c r="I15" s="7">
-        <v>8</v>
-      </c>
-      <c r="J15" s="59">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="8">
-        <v>8</v>
-      </c>
-      <c r="F16" s="8">
+      <c r="H20" s="6">
         <v>13</v>
       </c>
-      <c r="G16" s="8">
-        <v>5</v>
-      </c>
-      <c r="H16" s="8">
-        <v>8</v>
-      </c>
-      <c r="I16" s="8">
+      <c r="I20" s="6">
+        <v>8</v>
+      </c>
+      <c r="J20" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="10">
+        <v>8</v>
+      </c>
+      <c r="F21" s="8">
+        <v>5</v>
+      </c>
+      <c r="G21" s="8">
+        <v>8</v>
+      </c>
+      <c r="H21" s="8">
         <v>13</v>
       </c>
-      <c r="J16" s="59">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="9">
-        <v>5</v>
-      </c>
-      <c r="F17" s="9">
-        <v>8</v>
-      </c>
-      <c r="G17" s="9">
-        <v>8</v>
-      </c>
-      <c r="H17" s="9">
-        <v>8</v>
-      </c>
-      <c r="I17" s="9">
-        <v>5</v>
-      </c>
-      <c r="J17" s="59">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="54"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-    </row>
-    <row r="19" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="64"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="10">
-        <v>8</v>
-      </c>
-      <c r="F20" s="7">
+      <c r="I21" s="8">
+        <v>5</v>
+      </c>
+      <c r="J21" s="13">
+        <v>8</v>
+      </c>
+      <c r="K21" s="14"/>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="44"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+    </row>
+    <row r="23" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="43"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="11">
+        <v>8</v>
+      </c>
+      <c r="F24" s="9">
+        <v>8</v>
+      </c>
+      <c r="G24" s="6">
+        <v>8</v>
+      </c>
+      <c r="H24" s="6">
+        <v>8</v>
+      </c>
+      <c r="I24" s="6">
+        <v>8</v>
+      </c>
+      <c r="J24" s="13">
+        <v>8</v>
+      </c>
+      <c r="K24" s="14"/>
+    </row>
+    <row r="25" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="12">
         <v>13</v>
       </c>
-      <c r="G20" s="7">
-        <v>3</v>
-      </c>
-      <c r="H20" s="7">
+      <c r="F25" s="12">
+        <v>8</v>
+      </c>
+      <c r="G25" s="7">
+        <v>8</v>
+      </c>
+      <c r="H25" s="7">
         <v>13</v>
       </c>
-      <c r="I20" s="7">
-        <v>8</v>
-      </c>
-      <c r="J20" s="59">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="11">
-        <v>8</v>
-      </c>
-      <c r="F21" s="9">
-        <v>5</v>
-      </c>
-      <c r="G21" s="9">
-        <v>8</v>
-      </c>
-      <c r="H21" s="9">
-        <v>13</v>
-      </c>
-      <c r="I21" s="9">
-        <v>5</v>
-      </c>
-      <c r="J21" s="59">
-        <v>8</v>
-      </c>
-      <c r="K21" s="60"/>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
-    </row>
-    <row r="23" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="64"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="12">
-        <v>21</v>
-      </c>
-      <c r="F24" s="10">
-        <v>21</v>
-      </c>
-      <c r="G24" s="7">
-        <v>8</v>
-      </c>
-      <c r="H24" s="7">
-        <v>13</v>
-      </c>
-      <c r="I24" s="7">
-        <v>8</v>
-      </c>
-      <c r="J24" s="59">
-        <v>13</v>
-      </c>
-      <c r="K24" s="60"/>
-    </row>
-    <row r="25" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="13">
-        <v>13</v>
-      </c>
-      <c r="F25" s="13">
-        <v>13</v>
-      </c>
-      <c r="G25" s="8">
-        <v>8</v>
-      </c>
-      <c r="H25" s="8">
-        <v>13</v>
-      </c>
-      <c r="I25" s="8">
-        <v>8</v>
-      </c>
-      <c r="J25" s="59">
+      <c r="I25" s="7">
+        <v>8</v>
+      </c>
+      <c r="J25" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="27"/>
       <c r="E26" s="1">
-        <v>13</v>
-      </c>
-      <c r="F26" s="11">
-        <v>13</v>
-      </c>
-      <c r="G26" s="9">
-        <v>5</v>
-      </c>
-      <c r="H26" s="9">
-        <v>13</v>
-      </c>
-      <c r="I26" s="9">
-        <v>5</v>
-      </c>
-      <c r="J26" s="59">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="F26" s="10">
+        <v>5</v>
+      </c>
+      <c r="G26" s="8">
+        <v>5</v>
+      </c>
+      <c r="H26" s="8">
+        <v>5</v>
+      </c>
+      <c r="I26" s="8">
+        <v>5</v>
+      </c>
+      <c r="J26" s="13">
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
       <c r="E37" s="2"/>
     </row>
   </sheetData>

</xml_diff>